<commit_message>
Adding CCES NBHF detections to Tethys
NBHF detections are saved as "Odontoceti, Group: NBHG"
Updated detection worksheets to upload to Tethys
</commit_message>
<xml_diff>
--- a/Detection Worksheets/SWFSC_NBHF_effort.xlsx
+++ b/Detection Worksheets/SWFSC_NBHF_effort.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Group</t>
   </si>
@@ -44,52 +44,19 @@
     <t>Parameter 1</t>
   </si>
   <si>
-    <t>Parameter 2</t>
-  </si>
-  <si>
-    <t>Parameter 3</t>
-  </si>
-  <si>
-    <t>Parameter 4</t>
-  </si>
-  <si>
-    <t>Parameter 5</t>
-  </si>
-  <si>
-    <t>Parameter 6</t>
-  </si>
-  <si>
     <t>Other Odontocetes</t>
   </si>
   <si>
     <t>encounter</t>
   </si>
   <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>UO</t>
-  </si>
-  <si>
-    <t>peak 1 (low)</t>
-  </si>
-  <si>
-    <t>peak 2</t>
-  </si>
-  <si>
-    <t>peak 3</t>
-  </si>
-  <si>
-    <t>peak 4 (high)</t>
-  </si>
-  <si>
     <t>Clicks/&gt;100kHz</t>
   </si>
   <si>
-    <t>NBHF Odontocete</t>
+    <t>nClicks</t>
+  </si>
+  <si>
+    <t>NBHF</t>
   </si>
 </sst>
 </file>
@@ -429,13 +396,14 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="21.734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.9453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.20703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -458,55 +426,30 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">

</xml_diff>